<commit_message>
Cambios limpieza en los datos de Excel y cambios en diagrama de barras
</commit_message>
<xml_diff>
--- a/datos_estudiantes.xlsx
+++ b/datos_estudiantes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24822"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://espolec-my.sharepoint.com/personal/hroa_espol_edu_ec/Documents/ESPOL/Estadística/II2021/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\Proyectos\Estadistica\proyecto\ProyectoR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43F91ECB-B47F-41FD-B800-BB39C06DED51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06552723-663F-440E-844A-76AC6679B1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D75FBE2C-C027-4E05-B540-1CFC5D26FFD6}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$GA$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$GA$75</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -67,35 +67,35 @@
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{62DA466D-7FA5-4AC3-8126-FEA4C8C249BC}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     F
 M</t>
       </text>
     </comment>
     <comment ref="E1" authorId="1" shapeId="0" xr:uid="{B652994A-124F-41A6-BCB4-15D4E87881C7}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     libras</t>
       </text>
     </comment>
     <comment ref="K1" authorId="2" shapeId="0" xr:uid="{773EC9A8-C146-4C97-89CF-2A6C654457F2}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     1. Si
 2. No</t>
       </text>
     </comment>
     <comment ref="L1" authorId="3" shapeId="0" xr:uid="{861C5545-EF80-485F-866B-E1B926BDED5A}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     1. Ninguna
 2. 1 vez a la semana
 3. 2-3 veces a la semana
@@ -104,9 +104,9 @@
     </comment>
     <comment ref="M1" authorId="4" shapeId="0" xr:uid="{16DC081C-4B7F-44C1-89CB-3D027B19A571}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     1. Leve
 2. Moderada
 3. Alta</t>
@@ -114,17 +114,17 @@
     </comment>
     <comment ref="N1" authorId="5" shapeId="0" xr:uid="{72C54B92-1875-497B-99D0-105DFF4684F2}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     en minutos</t>
       </text>
     </comment>
     <comment ref="O1" authorId="6" shapeId="0" xr:uid="{BFD15A12-874D-46C5-936E-428CEA0615CA}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     1. En la mañana
 2. En la tarde
 3. En la noche</t>
@@ -132,78 +132,78 @@
     </comment>
     <comment ref="P1" authorId="7" shapeId="0" xr:uid="{A1AAAA96-A164-445E-B119-52D1885FC396}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     en litros</t>
       </text>
     </comment>
     <comment ref="Q1" authorId="8" shapeId="0" xr:uid="{8C086C8A-55BD-44DB-AC2E-67721EC1C2E0}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     en litros</t>
       </text>
     </comment>
     <comment ref="R1" authorId="9" shapeId="0" xr:uid="{E33689D3-6CA9-45DD-A0D9-39D6798DA9DA}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     en litros</t>
       </text>
     </comment>
     <comment ref="W1" authorId="10" shapeId="0" xr:uid="{631624D3-BDAD-463F-8121-CA6990B4EBB3}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     1. Si
 2. No</t>
       </text>
     </comment>
     <comment ref="X1" authorId="11" shapeId="0" xr:uid="{E0548FA5-6266-4324-A607-1E5BE68DA026}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     1. Si
 2. No</t>
       </text>
     </comment>
     <comment ref="Z1" authorId="12" shapeId="0" xr:uid="{96F48B23-4E16-409D-8FD7-B8B870E286BE}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     1. Si
 2. No</t>
       </text>
     </comment>
     <comment ref="AA1" authorId="13" shapeId="0" xr:uid="{D2034AED-CBBC-4762-8579-103320D5F77B}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     1. Si
 2. No</t>
       </text>
     </comment>
     <comment ref="AB1" authorId="14" shapeId="0" xr:uid="{B0EC0797-0817-43AA-A970-5BDA27E2C8DC}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     1. Si
 2. No</t>
       </text>
     </comment>
     <comment ref="AC1" authorId="15" shapeId="0" xr:uid="{94BE2BDF-2559-48B5-A7EF-FDE4AAABEACE}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     1. Ninguno o 1 episodio por semana
 2. 2 o 3 episodios por semana
 3. 4 o 5 episodios por semana
@@ -212,9 +212,9 @@
     </comment>
     <comment ref="AD1" authorId="16" shapeId="0" xr:uid="{3B95D1DE-1BA1-4672-8172-44C07A1A2D34}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     1. Ninguno o 1 episodio por semana
 2. 2 o 3 episodios por semana
 3. 4 o 5 episodios por semana
@@ -223,9 +223,9 @@
     </comment>
     <comment ref="AE1" authorId="17" shapeId="0" xr:uid="{30590A1D-19FB-46BF-B9AB-B5134E64E406}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     1. Ninguno o 1 episodio por semana
 2. 2 o 3 episodios por semana
 3. 4 o 5 episodios por semana
@@ -234,9 +234,9 @@
     </comment>
     <comment ref="AF1" authorId="18" shapeId="0" xr:uid="{BEBFDF81-BC50-4D70-BC3B-148327311972}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     1. Ninguno o 1 episodio por semana
 2. 2 o 3 episodios por semana
 3. 4 o 5 episodios por semana
@@ -245,9 +245,9 @@
     </comment>
     <comment ref="AG1" authorId="19" shapeId="0" xr:uid="{B5C452E3-0C62-4F60-B610-20A4F1D0223C}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     1. Ninguno o 1 episodio por semana
 2. 2 o 3 episodios por semana
 3. 4 o 5 episodios por semana
@@ -256,9 +256,9 @@
     </comment>
     <comment ref="AH1" authorId="20" shapeId="0" xr:uid="{603A4DAB-9866-4282-8F0A-9F9E87D8EBA3}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     1. Si
 2. No
 3. No sabe</t>
@@ -266,27 +266,27 @@
     </comment>
     <comment ref="AI1" authorId="21" shapeId="0" xr:uid="{3DE59A24-00B2-411C-8026-85D4B4A632A3}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     1. Si
 2. No</t>
       </text>
     </comment>
     <comment ref="AJ1" authorId="22" shapeId="0" xr:uid="{66291A3E-FD89-4738-8140-C70135F5DA13}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     1. Si
 2. No</t>
       </text>
     </comment>
     <comment ref="AK1" authorId="23" shapeId="0" xr:uid="{C42847A3-F706-4B74-AE9A-B040C7BFECC6}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     1. Fiebre
 2. Dolor de cabeza
 3. Dolor muscular
@@ -299,7 +299,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="84">
   <si>
     <t>Matricula</t>
   </si>
@@ -442,9 +442,6 @@
     <t>Química</t>
   </si>
   <si>
-    <t>w</t>
-  </si>
-  <si>
     <t>0?</t>
   </si>
   <si>
@@ -560,7 +557,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -684,7 +681,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1094,46 +1091,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5AF96B-391D-4437-92EB-22D84F72FFD0}">
-  <dimension ref="A1:GA75"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AK75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E56" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I80" sqref="I80"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="25.5546875" customWidth="1"/>
     <col min="11" max="11" width="8" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="18.109375" customWidth="1"/>
+    <col min="13" max="13" width="19.109375" customWidth="1"/>
     <col min="14" max="14" width="24" customWidth="1"/>
     <col min="15" max="15" width="20" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" customWidth="1"/>
+    <col min="16" max="16" width="18.6640625" customWidth="1"/>
     <col min="17" max="17" width="19" customWidth="1"/>
-    <col min="18" max="18" width="18.28515625" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" customWidth="1"/>
-    <col min="20" max="20" width="31.42578125" customWidth="1"/>
-    <col min="21" max="21" width="15.5703125" customWidth="1"/>
-    <col min="22" max="22" width="15.85546875" customWidth="1"/>
-    <col min="23" max="23" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.85546875" customWidth="1"/>
-    <col min="25" max="25" width="20.140625" customWidth="1"/>
-    <col min="26" max="26" width="15.7109375" customWidth="1"/>
-    <col min="27" max="27" width="18.140625" customWidth="1"/>
+    <col min="18" max="18" width="18.33203125" customWidth="1"/>
+    <col min="19" max="19" width="16.6640625" customWidth="1"/>
+    <col min="20" max="20" width="31.44140625" customWidth="1"/>
+    <col min="21" max="21" width="15.5546875" customWidth="1"/>
+    <col min="22" max="22" width="15.88671875" customWidth="1"/>
+    <col min="23" max="23" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.88671875" customWidth="1"/>
+    <col min="25" max="25" width="20.109375" customWidth="1"/>
+    <col min="26" max="26" width="15.6640625" customWidth="1"/>
+    <col min="27" max="27" width="18.109375" customWidth="1"/>
     <col min="29" max="29" width="18" customWidth="1"/>
-    <col min="30" max="30" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.44140625" customWidth="1"/>
     <col min="31" max="31" width="15" customWidth="1"/>
-    <col min="32" max="32" width="20.140625" customWidth="1"/>
-    <col min="33" max="33" width="20.28515625" customWidth="1"/>
-    <col min="36" max="36" width="11.42578125" customWidth="1"/>
-    <col min="37" max="37" width="11.85546875" customWidth="1"/>
+    <col min="32" max="32" width="20.109375" customWidth="1"/>
+    <col min="33" max="33" width="20.33203125" customWidth="1"/>
+    <col min="36" max="36" width="11.44140625" customWidth="1"/>
+    <col min="37" max="37" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:183" s="1" customFormat="1" ht="42.6" customHeight="1">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1246,7 +1244,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:183" s="9" customFormat="1" ht="15">
+    <row r="2" spans="1:37" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>202001400</v>
       </c>
@@ -1359,7 +1357,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:183">
+    <row r="3" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>202009569</v>
       </c>
@@ -1472,7 +1470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:183">
+    <row r="4" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>201914108</v>
       </c>
@@ -1576,7 +1574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:183">
+    <row r="5" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>202002648</v>
       </c>
@@ -1659,7 +1657,7 @@
         <v>2</v>
       </c>
       <c r="AE5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF5">
         <v>3</v>
@@ -1679,11 +1677,8 @@
       <c r="AK5">
         <v>1</v>
       </c>
-      <c r="GA5" t="s">
-        <v>47</v>
-      </c>
     </row>
-    <row r="6" spans="1:183">
+    <row r="6" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>202002010</v>
       </c>
@@ -1790,10 +1785,10 @@
         <v>2</v>
       </c>
       <c r="AK6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:183">
+    <row r="7" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>201701604</v>
       </c>
@@ -1822,7 +1817,7 @@
         <v>5</v>
       </c>
       <c r="J7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -1906,7 +1901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:183">
+    <row r="8" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>201803418</v>
       </c>
@@ -1926,7 +1921,7 @@
         <v>1.56</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H8">
         <v>7.61</v>
@@ -1935,7 +1930,7 @@
         <v>5</v>
       </c>
       <c r="J8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -2016,7 +2011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:183">
+    <row r="9" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>202000782</v>
       </c>
@@ -2045,7 +2040,7 @@
         <v>5</v>
       </c>
       <c r="J9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -2129,7 +2124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:183">
+    <row r="10" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>202008777</v>
       </c>
@@ -2242,7 +2237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:183">
+    <row r="11" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>202008744</v>
       </c>
@@ -2352,7 +2347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:183">
+    <row r="12" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>202003927</v>
       </c>
@@ -2381,7 +2376,7 @@
         <v>5</v>
       </c>
       <c r="J12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -2462,7 +2457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:183">
+    <row r="13" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>202005930</v>
       </c>
@@ -2491,7 +2486,7 @@
         <v>5</v>
       </c>
       <c r="J13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -2572,7 +2567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:183">
+    <row r="14" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>201904737</v>
       </c>
@@ -2601,7 +2596,7 @@
         <v>4</v>
       </c>
       <c r="J14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K14">
         <v>2</v>
@@ -2682,7 +2677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:183">
+    <row r="15" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>202005500</v>
       </c>
@@ -2699,7 +2694,7 @@
         <v>1.67</v>
       </c>
       <c r="G15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H15">
         <v>8.5399999999999991</v>
@@ -2708,7 +2703,7 @@
         <v>5</v>
       </c>
       <c r="J15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -2762,7 +2757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:183">
+    <row r="16" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>202007084</v>
       </c>
@@ -2782,7 +2777,7 @@
         <v>1.67</v>
       </c>
       <c r="G16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H16">
         <v>7.84</v>
@@ -2791,7 +2786,7 @@
         <v>4</v>
       </c>
       <c r="J16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -2872,7 +2867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>202000972</v>
       </c>
@@ -2889,7 +2884,7 @@
         <v>1.61</v>
       </c>
       <c r="G17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H17">
         <v>7.49</v>
@@ -2979,7 +2974,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>201915998</v>
       </c>
@@ -3008,7 +3003,7 @@
         <v>4</v>
       </c>
       <c r="J18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K18">
         <v>2</v>
@@ -3080,7 +3075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>202006045</v>
       </c>
@@ -3097,7 +3092,7 @@
         <v>1.56</v>
       </c>
       <c r="G19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H19">
         <v>8.26</v>
@@ -3106,7 +3101,7 @@
         <v>5</v>
       </c>
       <c r="J19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K19">
         <v>4</v>
@@ -3187,7 +3182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>201601549</v>
       </c>
@@ -3216,7 +3211,7 @@
         <v>4</v>
       </c>
       <c r="J20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -3300,7 +3295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>201608015</v>
       </c>
@@ -3329,7 +3324,7 @@
         <v>5</v>
       </c>
       <c r="J21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K21">
         <v>2</v>
@@ -3407,7 +3402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>201905148</v>
       </c>
@@ -3436,7 +3431,7 @@
         <v>5</v>
       </c>
       <c r="J22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K22">
         <v>2</v>
@@ -3511,7 +3506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>202011268</v>
       </c>
@@ -3540,7 +3535,7 @@
         <v>5</v>
       </c>
       <c r="J23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -3624,7 +3619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>202008801</v>
       </c>
@@ -3653,7 +3648,7 @@
         <v>5</v>
       </c>
       <c r="J24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K24">
         <v>1</v>
@@ -3737,7 +3732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>202002812</v>
       </c>
@@ -3766,7 +3761,7 @@
         <v>5</v>
       </c>
       <c r="J25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -3847,7 +3842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>202010633</v>
       </c>
@@ -3867,7 +3862,7 @@
         <v>1.5</v>
       </c>
       <c r="G26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H26">
         <v>7.88</v>
@@ -3876,7 +3871,7 @@
         <v>5</v>
       </c>
       <c r="J26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -3960,7 +3955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>201913654</v>
       </c>
@@ -3980,7 +3975,7 @@
         <v>1.78</v>
       </c>
       <c r="G27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H27">
         <v>7.43</v>
@@ -3989,7 +3984,7 @@
         <v>5</v>
       </c>
       <c r="J27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -4070,9 +4065,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
         <v>41</v>
@@ -4099,7 +4094,7 @@
         <v>5</v>
       </c>
       <c r="J28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K28">
         <v>1</v>
@@ -4183,7 +4178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>201913506</v>
       </c>
@@ -4212,7 +4207,7 @@
         <v>4</v>
       </c>
       <c r="J29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -4296,7 +4291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>202008892</v>
       </c>
@@ -4409,7 +4404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>202007241</v>
       </c>
@@ -4429,7 +4424,7 @@
         <v>1.69</v>
       </c>
       <c r="G31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H31">
         <v>8.3000000000000007</v>
@@ -4522,7 +4517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>202007738</v>
       </c>
@@ -4551,7 +4546,7 @@
         <v>4</v>
       </c>
       <c r="J32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K32">
         <v>1</v>
@@ -4608,19 +4603,19 @@
         <v>0</v>
       </c>
       <c r="AC32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD32">
         <v>2</v>
       </c>
       <c r="AE32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH32">
         <v>0</v>
@@ -4635,7 +4630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:37">
+    <row r="33" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>201912730</v>
       </c>
@@ -4655,7 +4650,7 @@
         <v>1.54</v>
       </c>
       <c r="G33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H33">
         <v>6.9</v>
@@ -4748,7 +4743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:37">
+    <row r="34" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>202009130</v>
       </c>
@@ -4858,7 +4853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:37">
+    <row r="35" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>201902244</v>
       </c>
@@ -4887,7 +4882,7 @@
         <v>4</v>
       </c>
       <c r="J35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K35">
         <v>1</v>
@@ -4968,7 +4963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:37">
+    <row r="36" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>202006235</v>
       </c>
@@ -5072,7 +5067,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:37">
+    <row r="37" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>202007902</v>
       </c>
@@ -5101,7 +5096,7 @@
         <v>5</v>
       </c>
       <c r="J37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K37">
         <v>4</v>
@@ -5158,19 +5153,19 @@
         <v>0</v>
       </c>
       <c r="AC37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH37">
         <v>0</v>
@@ -5185,7 +5180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:37">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>202006144</v>
       </c>
@@ -5205,7 +5200,7 @@
         <v>1.52</v>
       </c>
       <c r="G38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H38">
         <v>8.07</v>
@@ -5214,7 +5209,7 @@
         <v>5</v>
       </c>
       <c r="J38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K38">
         <v>1</v>
@@ -5298,7 +5293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:37">
+    <row r="39" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>201908167</v>
       </c>
@@ -5327,7 +5322,7 @@
         <v>4</v>
       </c>
       <c r="J39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K39">
         <v>1</v>
@@ -5408,7 +5403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:37">
+    <row r="40" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>201803806</v>
       </c>
@@ -5428,7 +5423,7 @@
         <v>1.67</v>
       </c>
       <c r="G40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H40">
         <v>7.26</v>
@@ -5437,7 +5432,7 @@
         <v>4</v>
       </c>
       <c r="J40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K40">
         <v>1</v>
@@ -5500,7 +5495,7 @@
         <v>2</v>
       </c>
       <c r="AE40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF40">
         <v>1</v>
@@ -5521,7 +5516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:37">
+    <row r="41" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>201909462</v>
       </c>
@@ -5631,7 +5626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:37">
+    <row r="42" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>201913613</v>
       </c>
@@ -5660,7 +5655,7 @@
         <v>5</v>
       </c>
       <c r="J42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K42">
         <v>2</v>
@@ -5735,7 +5730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:37">
+    <row r="43" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>201608395</v>
       </c>
@@ -5755,7 +5750,7 @@
         <v>1.65</v>
       </c>
       <c r="G43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H43">
         <v>7.4</v>
@@ -5764,7 +5759,7 @@
         <v>4</v>
       </c>
       <c r="J43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K43">
         <v>1</v>
@@ -5848,7 +5843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:37">
+    <row r="44" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>202011961</v>
       </c>
@@ -5877,7 +5872,7 @@
         <v>5</v>
       </c>
       <c r="J44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K44">
         <v>1</v>
@@ -5961,7 +5956,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:37">
+    <row r="45" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>201809597</v>
       </c>
@@ -5990,7 +5985,7 @@
         <v>6</v>
       </c>
       <c r="J45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K45">
         <v>1</v>
@@ -6068,7 +6063,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:37">
+    <row r="46" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>202007274</v>
       </c>
@@ -6097,7 +6092,7 @@
         <v>5</v>
       </c>
       <c r="J46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K46">
         <v>1</v>
@@ -6181,7 +6176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:37">
+    <row r="47" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>202011912</v>
       </c>
@@ -6210,7 +6205,7 @@
         <v>4</v>
       </c>
       <c r="J47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K47">
         <v>1</v>
@@ -6273,7 +6268,7 @@
         <v>2</v>
       </c>
       <c r="AE47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF47">
         <v>2</v>
@@ -6294,7 +6289,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:37">
+    <row r="48" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>201907268</v>
       </c>
@@ -6314,7 +6309,7 @@
         <v>1.8</v>
       </c>
       <c r="G48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H48">
         <v>8.16</v>
@@ -6323,7 +6318,7 @@
         <v>5</v>
       </c>
       <c r="J48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K48">
         <v>1</v>
@@ -6383,16 +6378,16 @@
         <v>1</v>
       </c>
       <c r="AD48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF48">
         <v>3</v>
       </c>
       <c r="AG48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH48">
         <v>3</v>
@@ -6407,7 +6402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:37">
+    <row r="49" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>201902749</v>
       </c>
@@ -6427,7 +6422,7 @@
         <v>1.7</v>
       </c>
       <c r="G49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H49">
         <v>8.35</v>
@@ -6436,7 +6431,7 @@
         <v>5</v>
       </c>
       <c r="J49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K49">
         <v>1</v>
@@ -6520,7 +6515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:37">
+    <row r="50" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>201914421</v>
       </c>
@@ -6549,7 +6544,7 @@
         <v>5</v>
       </c>
       <c r="J50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K50">
         <v>2</v>
@@ -6627,7 +6622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:37">
+    <row r="51" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>201906039</v>
       </c>
@@ -6647,7 +6642,7 @@
         <v>1.65</v>
       </c>
       <c r="G51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H51">
         <v>7.81</v>
@@ -6737,7 +6732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:37">
+    <row r="52" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>201907961</v>
       </c>
@@ -6766,7 +6761,7 @@
         <v>5</v>
       </c>
       <c r="J52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K52">
         <v>1</v>
@@ -6850,7 +6845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:37">
+    <row r="53" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>201913548</v>
       </c>
@@ -6879,7 +6874,7 @@
         <v>5</v>
       </c>
       <c r="J53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K53">
         <v>1</v>
@@ -6963,7 +6958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:37">
+    <row r="54" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="14">
         <v>202008306</v>
       </c>
@@ -6992,7 +6987,7 @@
         <v>5</v>
       </c>
       <c r="J54" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K54">
         <v>1</v>
@@ -7076,7 +7071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:37">
+    <row r="55" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>201912318</v>
       </c>
@@ -7096,7 +7091,7 @@
         <v>1.7</v>
       </c>
       <c r="G55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H55">
         <v>7.5</v>
@@ -7105,7 +7100,7 @@
         <v>5</v>
       </c>
       <c r="J55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K55">
         <v>2</v>
@@ -7180,7 +7175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:37">
+    <row r="56" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>202002010</v>
       </c>
@@ -7209,7 +7204,7 @@
         <v>5</v>
       </c>
       <c r="J56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K56">
         <v>1</v>
@@ -7293,7 +7288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:37">
+    <row r="57" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>202003018</v>
       </c>
@@ -7313,7 +7308,7 @@
         <v>1.5</v>
       </c>
       <c r="G57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H57">
         <v>7.75</v>
@@ -7322,7 +7317,7 @@
         <v>5</v>
       </c>
       <c r="J57" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K57">
         <v>1</v>
@@ -7406,7 +7401,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:37">
+    <row r="58" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>201916111</v>
       </c>
@@ -7435,7 +7430,7 @@
         <v>5</v>
       </c>
       <c r="J58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K58">
         <v>2</v>
@@ -7513,7 +7508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:37">
+    <row r="59" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>202003067</v>
       </c>
@@ -7542,7 +7537,7 @@
         <v>4</v>
       </c>
       <c r="J59" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K59">
         <v>1</v>
@@ -7626,7 +7621,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:37">
+    <row r="60" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>201605987</v>
       </c>
@@ -7655,7 +7650,7 @@
         <v>5</v>
       </c>
       <c r="J60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K60">
         <v>1</v>
@@ -7718,7 +7713,7 @@
         <v>1</v>
       </c>
       <c r="AE60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF60">
         <v>3</v>
@@ -7739,7 +7734,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:37">
+    <row r="61" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>202012878</v>
       </c>
@@ -7768,7 +7763,7 @@
         <v>4</v>
       </c>
       <c r="J61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K61">
         <v>2</v>
@@ -7843,7 +7838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:37">
+    <row r="62" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>202003489</v>
       </c>
@@ -7956,7 +7951,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:37">
+    <row r="63" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>201906187</v>
       </c>
@@ -7976,7 +7971,7 @@
         <v>1.69</v>
       </c>
       <c r="G63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H63">
         <v>7.69</v>
@@ -7985,7 +7980,7 @@
         <v>5</v>
       </c>
       <c r="J63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K63">
         <v>1</v>
@@ -8066,7 +8061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:37">
+    <row r="64" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>201915956</v>
       </c>
@@ -8095,7 +8090,7 @@
         <v>4</v>
       </c>
       <c r="J64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K64">
         <v>2</v>
@@ -8179,7 +8174,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:37">
+    <row r="65" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>202008124</v>
       </c>
@@ -8292,7 +8287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:37">
+    <row r="66" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>202009098</v>
       </c>
@@ -8321,7 +8316,7 @@
         <v>4</v>
       </c>
       <c r="J66" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K66">
         <v>1</v>
@@ -8405,7 +8400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:37">
+    <row r="67" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>201901535</v>
       </c>
@@ -8434,7 +8429,7 @@
         <v>5</v>
       </c>
       <c r="J67" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K67">
         <v>1</v>
@@ -8491,7 +8486,7 @@
         <v>2</v>
       </c>
       <c r="AC67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD67">
         <v>1</v>
@@ -8500,7 +8495,7 @@
         <v>1</v>
       </c>
       <c r="AF67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG67">
         <v>1</v>
@@ -8515,7 +8510,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:37">
+    <row r="68" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>201910742</v>
       </c>
@@ -8535,7 +8530,7 @@
         <v>1.69</v>
       </c>
       <c r="G68" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H68">
         <v>7.5</v>
@@ -8544,7 +8539,7 @@
         <v>5</v>
       </c>
       <c r="J68" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K68">
         <v>2</v>
@@ -8625,7 +8620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:37">
+    <row r="69" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>202004677</v>
       </c>
@@ -8654,7 +8649,7 @@
         <v>4</v>
       </c>
       <c r="J69" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K69">
         <v>1</v>
@@ -8738,7 +8733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:37">
+    <row r="70" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>202001863</v>
       </c>
@@ -8767,7 +8762,7 @@
         <v>5</v>
       </c>
       <c r="J70" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K70">
         <v>2</v>
@@ -8839,7 +8834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:37">
+    <row r="71" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>202009387</v>
       </c>
@@ -8952,7 +8947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:37">
+    <row r="72" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>201708898</v>
       </c>
@@ -8999,7 +8994,7 @@
         <v>2</v>
       </c>
       <c r="P72" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q72">
         <v>0</v>
@@ -9035,13 +9030,13 @@
         <v>0</v>
       </c>
       <c r="AC72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF72">
         <v>1</v>
@@ -9059,7 +9054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:37">
+    <row r="73" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>201912573</v>
       </c>
@@ -9088,7 +9083,7 @@
         <v>5</v>
       </c>
       <c r="J73" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K73">
         <v>1</v>
@@ -9172,7 +9167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:37">
+    <row r="74" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>202001228</v>
       </c>
@@ -9192,7 +9187,7 @@
         <v>1.7</v>
       </c>
       <c r="G74" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H74">
         <v>7.62</v>
@@ -9201,7 +9196,7 @@
         <v>5</v>
       </c>
       <c r="J74" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K74">
         <v>1</v>
@@ -9282,7 +9277,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:37">
+    <row r="75" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>201908753</v>
       </c>
@@ -9302,7 +9297,7 @@
         <v>1.63</v>
       </c>
       <c r="G75" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H75">
         <v>7.48</v>
@@ -9311,7 +9306,7 @@
         <v>5</v>
       </c>
       <c r="J75" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K75">
         <v>2</v>
@@ -9393,7 +9388,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:GA69" xr:uid="{2C5AF96B-391D-4437-92EB-22D84F72FFD0}"/>
+  <autoFilter ref="A1:GA75" xr:uid="{2C5AF96B-391D-4437-92EB-22D84F72FFD0}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="90"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Se elimino los datos de Frec. Semanal de Ejercicio
</commit_message>
<xml_diff>
--- a/datos_estudiantes.xlsx
+++ b/datos_estudiantes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Gomez\Desktop\proyectoestadisticaGithut\ProyectoR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Documents\Proyecto\Estadistica\ProyectoR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2531E79-A1E5-4C7C-8494-3E555E8F1756}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D965CD-7FBB-43D6-A4DA-DAA5EC7336CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D75FBE2C-C027-4E05-B540-1CFC5D26FFD6}"/>
+    <workbookView xWindow="4800" yWindow="0" windowWidth="14400" windowHeight="10200" xr2:uid="{D75FBE2C-C027-4E05-B540-1CFC5D26FFD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,439 +67,224 @@
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{62DA466D-7FA5-4AC3-8126-FEA4C8C249BC}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     F
 M</t>
-        </r>
       </text>
     </comment>
     <comment ref="E1" authorId="1" shapeId="0" xr:uid="{B652994A-124F-41A6-BCB4-15D4E87881C7}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     libras</t>
-        </r>
       </text>
     </comment>
     <comment ref="K1" authorId="2" shapeId="0" xr:uid="{773EC9A8-C146-4C97-89CF-2A6C654457F2}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1. Si
 2. No</t>
-        </r>
       </text>
     </comment>
     <comment ref="L1" authorId="3" shapeId="0" xr:uid="{861C5545-EF80-485F-866B-E1B926BDED5A}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1. Ninguna
 2. 1 vez a la semana
 3. 2-3 veces a la semana
 4. Más de 3 veces a la semana</t>
-        </r>
       </text>
     </comment>
     <comment ref="M1" authorId="4" shapeId="0" xr:uid="{16DC081C-4B7F-44C1-89CB-3D027B19A571}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1. Leve
 2. Moderada
 3. Alta</t>
-        </r>
       </text>
     </comment>
     <comment ref="N1" authorId="5" shapeId="0" xr:uid="{72C54B92-1875-497B-99D0-105DFF4684F2}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     en minutos</t>
-        </r>
       </text>
     </comment>
     <comment ref="O1" authorId="6" shapeId="0" xr:uid="{BFD15A12-874D-46C5-936E-428CEA0615CA}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1. En la mañana
 2. En la tarde
 3. En la noche</t>
-        </r>
       </text>
     </comment>
     <comment ref="P1" authorId="7" shapeId="0" xr:uid="{A1AAAA96-A164-445E-B119-52D1885FC396}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     en litros</t>
-        </r>
       </text>
     </comment>
     <comment ref="Q1" authorId="8" shapeId="0" xr:uid="{8C086C8A-55BD-44DB-AC2E-67721EC1C2E0}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     en litros</t>
-        </r>
       </text>
     </comment>
     <comment ref="R1" authorId="9" shapeId="0" xr:uid="{E33689D3-6CA9-45DD-A0D9-39D6798DA9DA}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     en litros</t>
-        </r>
       </text>
     </comment>
     <comment ref="W1" authorId="10" shapeId="0" xr:uid="{631624D3-BDAD-463F-8121-CA6990B4EBB3}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1. Si
 2. No</t>
-        </r>
       </text>
     </comment>
     <comment ref="X1" authorId="11" shapeId="0" xr:uid="{E0548FA5-6266-4324-A607-1E5BE68DA026}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1. Si
 2. No</t>
-        </r>
       </text>
     </comment>
     <comment ref="Z1" authorId="12" shapeId="0" xr:uid="{96F48B23-4E16-409D-8FD7-B8B870E286BE}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1. Si
 2. No</t>
-        </r>
       </text>
     </comment>
     <comment ref="AA1" authorId="13" shapeId="0" xr:uid="{D2034AED-CBBC-4762-8579-103320D5F77B}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1. Si
 2. No</t>
-        </r>
       </text>
     </comment>
     <comment ref="AB1" authorId="14" shapeId="0" xr:uid="{B0EC0797-0817-43AA-A970-5BDA27E2C8DC}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1. Si
 2. No</t>
-        </r>
       </text>
     </comment>
     <comment ref="AC1" authorId="15" shapeId="0" xr:uid="{94BE2BDF-2559-48B5-A7EF-FDE4AAABEACE}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1. Ninguno o 1 episodio por semana
 2. 2 o 3 episodios por semana
 3. 4 o 5 episodios por semana
 4. Más de 5 episodios por semana</t>
-        </r>
       </text>
     </comment>
     <comment ref="AD1" authorId="16" shapeId="0" xr:uid="{3B95D1DE-1BA1-4672-8172-44C07A1A2D34}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1. Ninguno o 1 episodio por semana
 2. 2 o 3 episodios por semana
 3. 4 o 5 episodios por semana
 4. Más de 5 episodios por semana</t>
-        </r>
       </text>
     </comment>
     <comment ref="AE1" authorId="17" shapeId="0" xr:uid="{30590A1D-19FB-46BF-B9AB-B5134E64E406}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1. Ninguno o 1 episodio por semana
 2. 2 o 3 episodios por semana
 3. 4 o 5 episodios por semana
 4. Más de 5 episodios por semana</t>
-        </r>
       </text>
     </comment>
     <comment ref="AF1" authorId="18" shapeId="0" xr:uid="{BEBFDF81-BC50-4D70-BC3B-148327311972}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1. Ninguno o 1 episodio por semana
 2. 2 o 3 episodios por semana
 3. 4 o 5 episodios por semana
 4. Más de 5 episodios por semana</t>
-        </r>
       </text>
     </comment>
     <comment ref="AG1" authorId="19" shapeId="0" xr:uid="{B5C452E3-0C62-4F60-B610-20A4F1D0223C}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1. Ninguno o 1 episodio por semana
 2. 2 o 3 episodios por semana
 3. 4 o 5 episodios por semana
 4. Más de 5 episodios por semana</t>
-        </r>
       </text>
     </comment>
     <comment ref="AH1" authorId="20" shapeId="0" xr:uid="{603A4DAB-9866-4282-8F0A-9F9E87D8EBA3}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1. Si
 2. No
 3. No sabe</t>
-        </r>
       </text>
     </comment>
     <comment ref="AI1" authorId="21" shapeId="0" xr:uid="{3DE59A24-00B2-411C-8026-85D4B4A632A3}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1. Si
 2. No</t>
-        </r>
       </text>
     </comment>
     <comment ref="AJ1" authorId="22" shapeId="0" xr:uid="{66291A3E-FD89-4738-8140-C70135F5DA13}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1. Si
 2. No</t>
-        </r>
       </text>
     </comment>
     <comment ref="AK1" authorId="23" shapeId="0" xr:uid="{C42847A3-F706-4B74-AE9A-B040C7BFECC6}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     1. Fiebre
@@ -507,7 +292,6 @@
 3. Dolor muscular
 4. Cansancio
 5. Sueño</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -515,7 +299,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="83">
   <si>
     <t>Matricula</t>
   </si>
@@ -761,9 +545,6 @@
   </si>
   <si>
     <t>Huaquillas</t>
-  </si>
-  <si>
-    <t>0.25</t>
   </si>
   <si>
     <t>Mecatronica</t>
@@ -1309,44 +1090,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5AF96B-391D-4437-92EB-22D84F72FFD0}">
   <dimension ref="A1:AK75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7265625" customWidth="1"/>
+    <col min="10" max="10" width="25.54296875" customWidth="1"/>
     <col min="11" max="11" width="8" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="18.1796875" customWidth="1"/>
+    <col min="13" max="13" width="19.1796875" customWidth="1"/>
     <col min="14" max="14" width="24" customWidth="1"/>
     <col min="15" max="15" width="20" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" customWidth="1"/>
+    <col min="16" max="16" width="18.7265625" customWidth="1"/>
     <col min="17" max="17" width="19" customWidth="1"/>
-    <col min="18" max="18" width="18.28515625" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" customWidth="1"/>
-    <col min="20" max="20" width="31.42578125" customWidth="1"/>
-    <col min="21" max="21" width="15.5703125" customWidth="1"/>
-    <col min="22" max="22" width="15.85546875" customWidth="1"/>
-    <col min="23" max="23" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.85546875" customWidth="1"/>
-    <col min="25" max="25" width="20.140625" customWidth="1"/>
-    <col min="26" max="26" width="15.7109375" customWidth="1"/>
-    <col min="27" max="27" width="18.140625" customWidth="1"/>
+    <col min="18" max="18" width="18.26953125" customWidth="1"/>
+    <col min="19" max="19" width="16.7265625" customWidth="1"/>
+    <col min="20" max="20" width="31.453125" customWidth="1"/>
+    <col min="21" max="21" width="15.54296875" customWidth="1"/>
+    <col min="22" max="22" width="15.81640625" customWidth="1"/>
+    <col min="23" max="23" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.81640625" customWidth="1"/>
+    <col min="25" max="25" width="20.1796875" customWidth="1"/>
+    <col min="26" max="26" width="15.7265625" customWidth="1"/>
+    <col min="27" max="27" width="18.1796875" customWidth="1"/>
     <col min="29" max="29" width="18" customWidth="1"/>
-    <col min="30" max="30" width="19.42578125" customWidth="1"/>
+    <col min="30" max="30" width="19.453125" customWidth="1"/>
     <col min="31" max="31" width="15" customWidth="1"/>
-    <col min="32" max="32" width="20.140625" customWidth="1"/>
-    <col min="33" max="33" width="20.28515625" customWidth="1"/>
-    <col min="36" max="36" width="11.42578125" customWidth="1"/>
-    <col min="37" max="37" width="11.85546875" customWidth="1"/>
+    <col min="32" max="32" width="20.1796875" customWidth="1"/>
+    <col min="33" max="33" width="20.26953125" customWidth="1"/>
+    <col min="36" max="36" width="11.453125" customWidth="1"/>
+    <col min="37" max="37" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="1" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1459,7 +1240,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9">
         <v>202001400</v>
       </c>
@@ -1572,7 +1353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>202009569</v>
       </c>
@@ -1685,7 +1466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>201914108</v>
       </c>
@@ -1789,7 +1570,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>202002648</v>
       </c>
@@ -1893,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>202002010</v>
       </c>
@@ -2003,7 +1784,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>201701604</v>
       </c>
@@ -2116,7 +1897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>201803418</v>
       </c>
@@ -2226,7 +2007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>202000782</v>
       </c>
@@ -2339,7 +2120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>202008777</v>
       </c>
@@ -2452,7 +2233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>202008744</v>
       </c>
@@ -2562,7 +2343,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>202003927</v>
       </c>
@@ -2672,7 +2453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>202005930</v>
       </c>
@@ -2782,7 +2563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>201904737</v>
       </c>
@@ -2892,7 +2673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>202005500</v>
       </c>
@@ -2972,7 +2753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>202007084</v>
       </c>
@@ -3082,7 +2863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>202000972</v>
       </c>
@@ -3189,7 +2970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>201915998</v>
       </c>
@@ -3290,7 +3071,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>202006045</v>
       </c>
@@ -3397,7 +3178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>201601549</v>
       </c>
@@ -3510,7 +3291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>201608015</v>
       </c>
@@ -3617,7 +3398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>201905148</v>
       </c>
@@ -3721,7 +3502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>202011268</v>
       </c>
@@ -3834,7 +3615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>202008801</v>
       </c>
@@ -3947,7 +3728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>202002812</v>
       </c>
@@ -4057,7 +3838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>202010633</v>
       </c>
@@ -4170,7 +3951,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>201913654</v>
       </c>
@@ -4280,7 +4061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -4393,7 +4174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>201913506</v>
       </c>
@@ -4506,7 +4287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>202008892</v>
       </c>
@@ -4619,7 +4400,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>202007241</v>
       </c>
@@ -4732,7 +4513,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>202007738</v>
       </c>
@@ -4845,7 +4626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>201912730</v>
       </c>
@@ -4958,7 +4739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>202009130</v>
       </c>
@@ -5068,7 +4849,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>201902244</v>
       </c>
@@ -5178,7 +4959,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>202006235</v>
       </c>
@@ -5282,7 +5063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>202007902</v>
       </c>
@@ -5395,7 +5176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>202006144</v>
       </c>
@@ -5508,7 +5289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>201908167</v>
       </c>
@@ -5618,7 +5399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>201803806</v>
       </c>
@@ -5731,7 +5512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>201909462</v>
       </c>
@@ -5841,7 +5622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>201913613</v>
       </c>
@@ -5945,7 +5726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>201608395</v>
       </c>
@@ -6058,7 +5839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>202011961</v>
       </c>
@@ -6171,7 +5952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>201809597</v>
       </c>
@@ -6278,7 +6059,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>202007274</v>
       </c>
@@ -6391,7 +6172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>202011912</v>
       </c>
@@ -6504,7 +6285,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>201907268</v>
       </c>
@@ -6617,7 +6398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>201902749</v>
       </c>
@@ -6730,7 +6511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>201914421</v>
       </c>
@@ -6837,7 +6618,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>201906039</v>
       </c>
@@ -6947,7 +6728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>201907961</v>
       </c>
@@ -7060,7 +6841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>201913548</v>
       </c>
@@ -7173,7 +6954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A54" s="14">
         <v>202008306</v>
       </c>
@@ -7286,7 +7067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>201912318</v>
       </c>
@@ -7390,7 +7171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>202002010</v>
       </c>
@@ -7503,7 +7284,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>202003018</v>
       </c>
@@ -7616,7 +7397,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>201916111</v>
       </c>
@@ -7723,7 +7504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>202003067</v>
       </c>
@@ -7836,7 +7617,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>201605987</v>
       </c>
@@ -7949,7 +7730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>202012878</v>
       </c>
@@ -8053,7 +7834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>202003489</v>
       </c>
@@ -8166,7 +7947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>201906187</v>
       </c>
@@ -8276,7 +8057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>201915956</v>
       </c>
@@ -8389,7 +8170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>202008124</v>
       </c>
@@ -8502,7 +8283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>202009098</v>
       </c>
@@ -8615,7 +8396,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>201901535</v>
       </c>
@@ -8725,7 +8506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>201910742</v>
       </c>
@@ -8835,7 +8616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>202004677</v>
       </c>
@@ -8948,7 +8729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>202001863</v>
       </c>
@@ -9049,7 +8830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>202009387</v>
       </c>
@@ -9162,7 +8943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>201708898</v>
       </c>
@@ -9208,8 +8989,8 @@
       <c r="O72">
         <v>2</v>
       </c>
-      <c r="P72" t="s">
-        <v>82</v>
+      <c r="P72">
+        <v>0.25</v>
       </c>
       <c r="Q72">
         <v>0</v>
@@ -9269,7 +9050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>201912573</v>
       </c>
@@ -9298,7 +9079,7 @@
         <v>5</v>
       </c>
       <c r="J73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K73">
         <v>1</v>
@@ -9382,7 +9163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>202001228</v>
       </c>
@@ -9492,7 +9273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>201908753</v>
       </c>

</xml_diff>